<commit_message>
Tabela Final com a informação sobre genes/proteínas
</commit_message>
<xml_diff>
--- a/Resultados/Tabela/Tabela Final.xlsx
+++ b/Resultados/Tabela/Tabela Final.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Varzim\Documents\GitHub\Trab_Lab_Algoritmos\Resultados\Tabela\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4650"/>
   </bookViews>
@@ -11990,7 +11985,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12000,8 +11995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A227" sqref="A227:XFD227"/>
+    <sheetView tabSelected="1" topLeftCell="O64" workbookViewId="0">
+      <selection activeCell="O152" sqref="A152:XFD152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12357,7 +12352,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="72" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>99</v>
       </c>
@@ -15557,7 +15552,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="84" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:22" ht="72" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>997</v>
       </c>
@@ -19331,7 +19326,7 @@
         <v>2052</v>
       </c>
     </row>
-    <row r="123" spans="1:22" ht="60" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>2053</v>
       </c>
@@ -20847,7 +20842,7 @@
       <c r="U148" s="12"/>
       <c r="V148" s="5"/>
     </row>
-    <row r="149" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:22" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
         <v>2473</v>
       </c>
@@ -20971,7 +20966,7 @@
         <v>2508</v>
       </c>
     </row>
-    <row r="151" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:22" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
         <v>2509</v>
       </c>
@@ -21037,7 +21032,7 @@
         <v>2528</v>
       </c>
     </row>
-    <row r="152" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:22" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
         <v>2529</v>
       </c>
@@ -22241,7 +22236,7 @@
         <v>2857</v>
       </c>
     </row>
-    <row r="173" spans="1:22" ht="48" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:22" ht="36" x14ac:dyDescent="0.2">
       <c r="A173" s="5" t="s">
         <v>2858</v>
       </c>
@@ -24565,7 +24560,7 @@
         <v>3512</v>
       </c>
     </row>
-    <row r="212" spans="1:22" ht="84" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:22" ht="72" x14ac:dyDescent="0.2">
       <c r="A212" s="5" t="s">
         <v>3513</v>
       </c>

</xml_diff>